<commit_message>
4_Sort_0s_1s_2s solved in python
</commit_message>
<xml_diff>
--- a/SAMYAK/LOVE BABBAR SHEET/FINAL450.xlsx
+++ b/SAMYAK/LOVE BABBAR SHEET/FINAL450.xlsx
@@ -1704,12 +1704,12 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="123"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.84"/>

</xml_diff>